<commit_message>
Remodelling code making use of the BrokenLink class.
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/Github/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1AD8619-4C0D-9843-AE50-15B9164523A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F1F5BE-4B35-DC46-9CDA-0E6C5B3A0F67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,52 +25,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Status Code</t>
+  </si>
+  <si>
+    <t>Content Type</t>
+  </si>
+  <si>
+    <t>Response Time</t>
+  </si>
+  <si>
+    <t>Header Location</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
     <t>Internal/External</t>
   </si>
   <si>
-    <t>Origin</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Status Code</t>
-  </si>
-  <si>
-    <t>Content Type</t>
-  </si>
-  <si>
-    <t>Response Time</t>
-  </si>
-  <si>
-    <t>Header Location</t>
-  </si>
-  <si>
-    <t>Error Message</t>
-  </si>
-  <si>
     <t>Some</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>fill</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>excel</t>
-  </si>
-  <si>
-    <t>sheet</t>
   </si>
 </sst>
 </file>
@@ -119,12 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,9 +467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -480,263 +486,266 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+      <c r="A2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
+      <c r="A3" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
+      <c r="A4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
+      <c r="A5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
+      <c r="A6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
+      <c r="A8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
+      <c r="A10" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Only have excel file in ram instead of saving into egg cache
With this change the excel workbook will not be saved physically
anymore but in ram only.
Also I added a better output to the excel sheet comparing test showing
the diff of the two dataframes loaded from the excel workbooks.
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/Github/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F1F5BE-4B35-DC46-9CDA-0E6C5B3A0F67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032E2221-0570-1E4B-9A90-071BB375FE50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Remove header location from excel report
Since the link report does not show any pages being successful, we do
not get any header location in all cases tested. Therefore we can remove
this column in the report.
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/Github/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032E2221-0570-1E4B-9A90-071BB375FE50}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CAA9F-3CC1-894C-8104-231F21FBFE79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
   <si>
     <t>Origin</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Response Time</t>
   </si>
   <si>
-    <t>Header Location</t>
-  </si>
-  <si>
     <t>Error Message</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>the</t>
-  </si>
-  <si>
-    <t>excel</t>
   </si>
   <si>
     <t>sheet</t>
@@ -467,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -479,14 +473,12 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="11" width="20.6640625" customWidth="1"/>
+    <col min="6" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -506,249 +498,219 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new column creator to excel workbook
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/Github/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/PythonProjects/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CAA9F-3CC1-894C-8104-231F21FBFE79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A258D-5459-3D44-8A50-402C8D2B8BB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>Origin</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Some</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>slowly</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -476,7 +482,7 @@
     <col min="6" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -498,8 +504,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -521,8 +530,11 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -544,8 +556,11 @@
       <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -567,8 +582,11 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -590,8 +608,11 @@
       <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -613,8 +634,11 @@
       <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -636,8 +660,11 @@
       <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -659,8 +686,11 @@
       <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -682,8 +712,11 @@
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -705,8 +738,11 @@
       <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add workflow state column.
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/PythonProjects/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A258D-5459-3D44-8A50-402C8D2B8BB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C217F85-03EB-7041-927F-A019A8D45C23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>Origin</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>slowly</t>
+  </si>
+  <si>
+    <t>Workflow State</t>
+  </si>
+  <si>
+    <t>man!</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,7 +488,7 @@
     <col min="6" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -507,8 +513,11 @@
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -533,8 +542,11 @@
       <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -559,8 +571,11 @@
       <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -585,8 +600,11 @@
       <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -611,8 +629,11 @@
       <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -637,8 +658,11 @@
       <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -663,8 +687,11 @@
       <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -689,8 +716,11 @@
       <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -715,8 +745,11 @@
       <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -741,8 +774,11 @@
       <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put review state in report instead of workflow and adapt tests.
</commit_message>
<xml_diff>
--- a/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
+++ b/ftw/linkchecker/tests/exemplar_data/expected_excel_sheet_outcome.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/busykoala/Documents/PythonProjects/ftw.linkchecker/ftw/linkchecker/tests/exemplar_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C217F85-03EB-7041-927F-A019A8D45C23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A348FF-FCEC-4B4B-BE66-B404749A1BB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,10 +73,10 @@
     <t>slowly</t>
   </si>
   <si>
-    <t>Workflow State</t>
-  </si>
-  <si>
     <t>man!</t>
+  </si>
+  <si>
+    <t>Review State</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,7 +514,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -572,7 +572,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -601,7 +601,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -630,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -659,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -717,7 +717,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>15</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>